<commit_message>
updates on iteration 4 docs and meeting risks
</commit_message>
<xml_diff>
--- a/Documentation/8.0 Risk Assessment/Risk Management Log v2.3.xlsx
+++ b/Documentation/8.0 Risk Assessment/Risk Management Log v2.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38200" windowHeight="19260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t xml:space="preserve">Risk ID </t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>We have implemented a pin code that would need to be entered in manually, mitigating the risk of someone being able to technically attack it. Although this is still subject to social engineering attacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email only allows 10 bounces a day </t>
+  </si>
+  <si>
+    <t>We validate all emails using javaScript</t>
   </si>
 </sst>
 </file>
@@ -664,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -756,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H22" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H23" si="0">F4*G4</f>
         <v>10</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -779,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f t="shared" ref="C5:C22" si="1">IF(H5&lt;=7, "Low Risk",IF(H5&gt;=17,"High Risk","Medium Risk"))</f>
+        <f t="shared" ref="C5:C23" si="1">IF(H5&lt;=7, "Low Risk",IF(H5&gt;=17,"High Risk","Medium Risk"))</f>
         <v>Low Risk</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1412,9 +1418,7 @@
       <c r="K20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L20" s="7">
-        <v>41957</v>
-      </c>
+      <c r="L20" s="7"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
@@ -1504,16 +1508,38 @@
       <c r="B23" s="8">
         <v>20</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="7"/>
+      <c r="C23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Medium Risk</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="5">
+        <v>3</v>
+      </c>
+      <c r="G23" s="5">
+        <v>4</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23" s="7">
+        <v>41992</v>
+      </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>

</xml_diff>